<commit_message>
code, plots and notes
</commit_message>
<xml_diff>
--- a/Data/GP2_BODYWEIGHT.xlsx
+++ b/Data/GP2_BODYWEIGHT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Guinea-Pig-data_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69DE870-D306-43C4-B15A-CE0C829CF462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E67A55-D03D-430C-86FF-35C15AF94524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{BC909284-01A5-4060-BFAF-EA7D13221CD6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BC909284-01A5-4060-BFAF-EA7D13221CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -79,18 +79,6 @@
   <si>
     <t>Weekly_weight</t>
   </si>
-  <si>
-    <t>ADG</t>
-  </si>
-  <si>
-    <t>W2</t>
-  </si>
-  <si>
-    <t>W3</t>
-  </si>
-  <si>
-    <t>ADG3</t>
-  </si>
 </sst>
 </file>
 
@@ -105,18 +93,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,12 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -473,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED2772E-737C-40C6-A55D-2BB763B852CE}">
-  <dimension ref="A1:N794"/>
+  <dimension ref="A1:G794"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,10 +463,9 @@
     <col min="1" max="5" width="8.7265625" style="1"/>
     <col min="6" max="6" width="13.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -509,20 +487,8 @@
       <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -544,22 +510,8 @@
       <c r="G2" s="1">
         <v>216</v>
       </c>
-      <c r="H2" s="2">
-        <f>G2-F2</f>
-        <v>-89</v>
-      </c>
-      <c r="L2">
-        <v>435</v>
-      </c>
-      <c r="M2">
-        <v>484</v>
-      </c>
-      <c r="N2">
-        <f>M2-L2</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -581,22 +533,8 @@
       <c r="G3" s="1">
         <v>368</v>
       </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H21" si="0">G3-F3</f>
-        <v>63</v>
-      </c>
-      <c r="L3">
-        <v>408</v>
-      </c>
-      <c r="M3">
-        <v>450</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N21" si="1">M3-L3</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -618,22 +556,8 @@
       <c r="G4" s="1">
         <v>511</v>
       </c>
-      <c r="H4" s="2">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="L4">
-        <v>510</v>
-      </c>
-      <c r="M4">
-        <v>537</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -655,22 +579,8 @@
       <c r="G5" s="1">
         <v>389</v>
       </c>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>224</v>
-      </c>
-      <c r="L5">
-        <v>245</v>
-      </c>
-      <c r="M5">
-        <v>268</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -692,22 +602,8 @@
       <c r="G6" s="1">
         <v>382</v>
       </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="L6">
-        <v>432</v>
-      </c>
-      <c r="M6">
-        <v>485</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -729,22 +625,8 @@
       <c r="G7" s="1">
         <v>617</v>
       </c>
-      <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="L7">
-        <v>638</v>
-      </c>
-      <c r="M7">
-        <v>672</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -766,22 +648,8 @@
       <c r="G8" s="1">
         <v>536</v>
       </c>
-      <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L8">
-        <v>504</v>
-      </c>
-      <c r="M8">
-        <v>488</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="1"/>
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -803,22 +671,8 @@
       <c r="G9" s="1">
         <v>634</v>
       </c>
-      <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="L9">
-        <v>641</v>
-      </c>
-      <c r="M9">
-        <v>671</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -840,22 +694,8 @@
       <c r="G10" s="1">
         <v>512</v>
       </c>
-      <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="L10">
-        <v>524</v>
-      </c>
-      <c r="M10">
-        <v>569</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -877,22 +717,8 @@
       <c r="G11" s="1">
         <v>548</v>
       </c>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="L11">
-        <v>520</v>
-      </c>
-      <c r="M11">
-        <v>551</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -914,22 +740,8 @@
       <c r="G12" s="1">
         <v>504</v>
       </c>
-      <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="L12">
-        <v>521</v>
-      </c>
-      <c r="M12">
-        <v>559</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -951,22 +763,8 @@
       <c r="G13" s="1">
         <v>561</v>
       </c>
-      <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="L13">
-        <v>586</v>
-      </c>
-      <c r="M13">
-        <v>624</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -988,22 +786,8 @@
       <c r="G14" s="1">
         <v>514</v>
       </c>
-      <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="L14">
-        <v>503</v>
-      </c>
-      <c r="M14">
-        <v>507</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1025,22 +809,8 @@
       <c r="G15" s="1">
         <v>578</v>
       </c>
-      <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="L15">
-        <v>593</v>
-      </c>
-      <c r="M15">
-        <v>627</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1062,22 +832,8 @@
       <c r="G16" s="1">
         <v>635</v>
       </c>
-      <c r="H16" s="2">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="L16">
-        <v>672</v>
-      </c>
-      <c r="M16">
-        <v>702</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1099,22 +855,8 @@
       <c r="G17" s="1">
         <v>372</v>
       </c>
-      <c r="H17" s="2">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="L17">
-        <v>416</v>
-      </c>
-      <c r="M17">
-        <v>465</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1136,22 +878,8 @@
       <c r="G18" s="1">
         <v>635</v>
       </c>
-      <c r="H18" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L18">
-        <v>633</v>
-      </c>
-      <c r="M18">
-        <v>633</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1173,22 +901,8 @@
       <c r="G19" s="1">
         <v>712</v>
       </c>
-      <c r="H19" s="2">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-      <c r="L19">
-        <v>783</v>
-      </c>
-      <c r="M19">
-        <v>826</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1210,22 +924,8 @@
       <c r="G20" s="1">
         <v>499</v>
       </c>
-      <c r="H20" s="2">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="L20">
-        <v>555</v>
-      </c>
-      <c r="M20">
-        <v>611</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1247,22 +947,8 @@
       <c r="G21" s="1">
         <v>403</v>
       </c>
-      <c r="H21" s="2">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="L21">
-        <v>500</v>
-      </c>
-      <c r="M21">
-        <v>526</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1284,11 +970,8 @@
       <c r="G22" s="1">
         <v>435</v>
       </c>
-      <c r="H22" s="2">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1310,11 +993,8 @@
       <c r="G23" s="1">
         <v>408</v>
       </c>
-      <c r="H23" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1336,11 +1016,8 @@
       <c r="G24" s="1">
         <v>510</v>
       </c>
-      <c r="H24" s="2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1362,11 +1039,8 @@
       <c r="G25" s="1">
         <v>245</v>
       </c>
-      <c r="H25" s="2">
-        <v>-144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1388,11 +1062,8 @@
       <c r="G26" s="1">
         <v>432</v>
       </c>
-      <c r="H26" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1414,11 +1085,8 @@
       <c r="G27" s="1">
         <v>638</v>
       </c>
-      <c r="H27" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -1440,11 +1108,8 @@
       <c r="G28" s="1">
         <v>504</v>
       </c>
-      <c r="H28" s="2">
-        <v>-32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1466,11 +1131,8 @@
       <c r="G29" s="1">
         <v>641</v>
       </c>
-      <c r="H29" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -1492,11 +1154,8 @@
       <c r="G30" s="1">
         <v>524</v>
       </c>
-      <c r="H30" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -1518,11 +1177,8 @@
       <c r="G31" s="1">
         <v>520</v>
       </c>
-      <c r="H31" s="2">
-        <v>-28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1544,11 +1200,8 @@
       <c r="G32" s="1">
         <v>521</v>
       </c>
-      <c r="H32" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -1570,11 +1223,8 @@
       <c r="G33" s="1">
         <v>586</v>
       </c>
-      <c r="H33" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>1</v>
       </c>
@@ -1596,11 +1246,8 @@
       <c r="G34" s="1">
         <v>503</v>
       </c>
-      <c r="H34" s="2">
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1622,11 +1269,8 @@
       <c r="G35" s="1">
         <v>593</v>
       </c>
-      <c r="H35" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -1648,11 +1292,8 @@
       <c r="G36" s="1">
         <v>672</v>
       </c>
-      <c r="H36" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>1</v>
       </c>
@@ -1674,11 +1315,8 @@
       <c r="G37" s="1">
         <v>416</v>
       </c>
-      <c r="H37" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -1700,11 +1338,8 @@
       <c r="G38" s="1">
         <v>633</v>
       </c>
-      <c r="H38" s="2">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -1726,11 +1361,8 @@
       <c r="G39" s="1">
         <v>783</v>
       </c>
-      <c r="H39" s="2">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -1752,11 +1384,8 @@
       <c r="G40" s="1">
         <v>555</v>
       </c>
-      <c r="H40" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -1778,11 +1407,8 @@
       <c r="G41" s="1">
         <v>500</v>
       </c>
-      <c r="H41" s="2">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -1804,11 +1430,8 @@
       <c r="G42" s="1">
         <v>484</v>
       </c>
-      <c r="H42" s="2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -1830,11 +1453,8 @@
       <c r="G43" s="1">
         <v>450</v>
       </c>
-      <c r="H43" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -1856,11 +1476,8 @@
       <c r="G44" s="1">
         <v>537</v>
       </c>
-      <c r="H44" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -1882,11 +1499,8 @@
       <c r="G45" s="1">
         <v>268</v>
       </c>
-      <c r="H45" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -1908,11 +1522,8 @@
       <c r="G46" s="1">
         <v>485</v>
       </c>
-      <c r="H46" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -1934,11 +1545,8 @@
       <c r="G47" s="1">
         <v>672</v>
       </c>
-      <c r="H47" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -1960,11 +1568,8 @@
       <c r="G48" s="1">
         <v>488</v>
       </c>
-      <c r="H48" s="2">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -1986,11 +1591,8 @@
       <c r="G49" s="1">
         <v>671</v>
       </c>
-      <c r="H49" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -2012,11 +1614,8 @@
       <c r="G50" s="1">
         <v>569</v>
       </c>
-      <c r="H50" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -2038,11 +1637,8 @@
       <c r="G51" s="1">
         <v>551</v>
       </c>
-      <c r="H51" s="2">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>1</v>
       </c>
@@ -2064,11 +1660,8 @@
       <c r="G52" s="1">
         <v>559</v>
       </c>
-      <c r="H52" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>1</v>
       </c>
@@ -2090,11 +1683,8 @@
       <c r="G53" s="1">
         <v>624</v>
       </c>
-      <c r="H53" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>1</v>
       </c>
@@ -2116,11 +1706,8 @@
       <c r="G54" s="1">
         <v>507</v>
       </c>
-      <c r="H54" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>1</v>
       </c>
@@ -2142,11 +1729,8 @@
       <c r="G55" s="1">
         <v>627</v>
       </c>
-      <c r="H55" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>1</v>
       </c>
@@ -2168,11 +1752,8 @@
       <c r="G56" s="1">
         <v>702</v>
       </c>
-      <c r="H56" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>1</v>
       </c>
@@ -2194,11 +1775,8 @@
       <c r="G57" s="1">
         <v>465</v>
       </c>
-      <c r="H57" s="2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>1</v>
       </c>
@@ -2220,11 +1798,8 @@
       <c r="G58" s="1">
         <v>633</v>
       </c>
-      <c r="H58" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>1</v>
       </c>
@@ -2246,11 +1821,8 @@
       <c r="G59" s="1">
         <v>826</v>
       </c>
-      <c r="H59" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>1</v>
       </c>
@@ -2272,11 +1844,8 @@
       <c r="G60" s="1">
         <v>611</v>
       </c>
-      <c r="H60" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>1</v>
       </c>
@@ -2298,11 +1867,8 @@
       <c r="G61" s="1">
         <v>526</v>
       </c>
-      <c r="H61" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>1</v>
       </c>
@@ -2325,7 +1891,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>1</v>
       </c>
@@ -2348,7 +1914,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>1</v>
       </c>

</xml_diff>